<commit_message>
Update for May metrics
</commit_message>
<xml_diff>
--- a/Code/Output/August_2021/Metrics_Report_August_2021.xlsx
+++ b/Code/Output/August_2021/Metrics_Report_August_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.52\home$\BryanP\Projects\project_files\USAI\Code\Output\August_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EFA8BF-13A4-4853-A4DD-012D6E0B9D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C05F13-AC6D-4AD6-ACCE-172C4D5F2821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11295" yWindow="2400" windowWidth="13515" windowHeight="10545" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7155" yWindow="2970" windowWidth="12945" windowHeight="11505" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver and Engine RMAs" sheetId="3" r:id="rId1"/>
@@ -672,15 +672,38 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="5">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="\+0;\-0;0"/>
     <numFmt numFmtId="166" formatCode="\+&quot;$&quot;0.00;\-&quot;$&quot;0.00;&quot;$&quot;0.00"/>
   </numFmts>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1569,51 +1592,111 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="164">
+  <cellStyleXfs count="224">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1735,7 +1818,7 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1747,16 +1830,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1779,10 +1862,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="21" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1791,7 +1874,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1806,14 +1889,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1831,7 +1914,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1840,19 +1923,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1871,7 +1954,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1881,10 +1964,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1905,15 +1988,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1934,7 +2017,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1949,11 +2032,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1983,7 +2066,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1992,19 +2075,19 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="12" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2022,14 +2105,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="44"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="64"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="64" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="84"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="84"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="124"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="124" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="44"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="64"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="64" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="84"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="84"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="124"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="124" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="144"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="144" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="164"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="164"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="164"/>
+    <xf numFmtId="8" fontId="3" fillId="0" borderId="0" xfId="164" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="184"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="184"/>
+    <xf numFmtId="6" fontId="2" fillId="0" borderId="0" xfId="184" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2038,187 +2130,242 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="144"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="144" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="204" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="164">
+  <cellStyles count="224">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1 10" xfId="206" xr:uid="{DF50A6DA-51F4-4649-A970-1DA017078481}"/>
     <cellStyle name="20% - Accent1 2" xfId="46" xr:uid="{02BAB7D6-C846-4D2A-912F-3C07D1DD4FF0}"/>
     <cellStyle name="20% - Accent1 3" xfId="66" xr:uid="{89DAF94E-6BDD-4FDC-8302-85528D01EDDA}"/>
     <cellStyle name="20% - Accent1 4" xfId="86" xr:uid="{7B1B9CF1-2737-409F-9F4B-CF269FE4FDDC}"/>
     <cellStyle name="20% - Accent1 5" xfId="106" xr:uid="{D383746A-2627-40CF-97D3-5DCD766843EB}"/>
     <cellStyle name="20% - Accent1 6" xfId="126" xr:uid="{B9AA82B2-161B-49C0-A326-202F08A5DFBA}"/>
     <cellStyle name="20% - Accent1 7" xfId="146" xr:uid="{49C936C6-9356-47D9-98D3-88AA5D55184F}"/>
+    <cellStyle name="20% - Accent1 8" xfId="166" xr:uid="{C1A94D54-1B88-4E95-9B93-F7F16659E368}"/>
+    <cellStyle name="20% - Accent1 9" xfId="186" xr:uid="{828F0CCF-A5FB-41F5-A50C-15B3F2AD3681}"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2 10" xfId="209" xr:uid="{353E4B0F-184A-4559-AD5C-E36749E4BA01}"/>
     <cellStyle name="20% - Accent2 2" xfId="49" xr:uid="{9B8B4624-16AD-4AEE-A198-A8FDF7C8BD81}"/>
     <cellStyle name="20% - Accent2 3" xfId="69" xr:uid="{7FC42DE8-97E3-483D-86E4-1C43881206A5}"/>
     <cellStyle name="20% - Accent2 4" xfId="89" xr:uid="{6C52E251-C353-4B7E-A4FD-FEA2151429DF}"/>
     <cellStyle name="20% - Accent2 5" xfId="109" xr:uid="{92EB08E7-89C8-4BB5-B15F-98FC790C0D4D}"/>
     <cellStyle name="20% - Accent2 6" xfId="129" xr:uid="{71241A39-D173-4A8A-A652-0EFAE10EE26A}"/>
     <cellStyle name="20% - Accent2 7" xfId="149" xr:uid="{FBFFBFE1-EEBE-4858-B5A3-1B43AABF891E}"/>
+    <cellStyle name="20% - Accent2 8" xfId="169" xr:uid="{217D5503-B776-42D0-AC7D-298115F8A650}"/>
+    <cellStyle name="20% - Accent2 9" xfId="189" xr:uid="{25DA9A39-C24C-4FCE-B979-9672B8D52ADC}"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3 10" xfId="212" xr:uid="{43782D75-7626-4192-A3D3-600A95743F12}"/>
     <cellStyle name="20% - Accent3 2" xfId="52" xr:uid="{7A856016-D5DC-4F33-97B8-3BDEC6B41FAE}"/>
     <cellStyle name="20% - Accent3 3" xfId="72" xr:uid="{21E79185-8EAF-4DAB-8BA0-96D4426D8503}"/>
     <cellStyle name="20% - Accent3 4" xfId="92" xr:uid="{8ACA4BD6-058B-4C3C-9972-E65B16B05DA4}"/>
     <cellStyle name="20% - Accent3 5" xfId="112" xr:uid="{39CB54AD-B1F7-4A88-AD5B-8643D11AFAE2}"/>
     <cellStyle name="20% - Accent3 6" xfId="132" xr:uid="{5749F878-D763-4038-B2A5-2F956162E572}"/>
     <cellStyle name="20% - Accent3 7" xfId="152" xr:uid="{A9D32BF4-30AB-475E-AE9E-003F97B454BA}"/>
+    <cellStyle name="20% - Accent3 8" xfId="172" xr:uid="{E881B821-D535-44CD-B98F-0538641C94ED}"/>
+    <cellStyle name="20% - Accent3 9" xfId="192" xr:uid="{CA66F180-AC36-4C6F-B239-7C7A0741F272}"/>
     <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4 10" xfId="215" xr:uid="{490FD692-A5BE-4B6C-8F99-87E51B4A63D9}"/>
     <cellStyle name="20% - Accent4 2" xfId="55" xr:uid="{27A713D1-8C98-4F40-882E-CF4BF70BE480}"/>
     <cellStyle name="20% - Accent4 3" xfId="75" xr:uid="{D490D1A2-E23D-45F5-AA9B-7EE9492D3575}"/>
     <cellStyle name="20% - Accent4 4" xfId="95" xr:uid="{56AD7626-24AD-4771-AE7E-62818455D23E}"/>
     <cellStyle name="20% - Accent4 5" xfId="115" xr:uid="{791806D0-07AB-479A-ACAB-ED64722479C2}"/>
     <cellStyle name="20% - Accent4 6" xfId="135" xr:uid="{1878D8B9-4DD7-4321-98E6-54BF9A277026}"/>
     <cellStyle name="20% - Accent4 7" xfId="155" xr:uid="{2460F179-8B2B-42C7-80F7-A4DC7F653209}"/>
+    <cellStyle name="20% - Accent4 8" xfId="175" xr:uid="{594DAF39-9829-459F-93B4-D56D7DF47161}"/>
+    <cellStyle name="20% - Accent4 9" xfId="195" xr:uid="{7B0BBE92-C334-46BA-ADD3-B2AC27239F58}"/>
     <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5 10" xfId="218" xr:uid="{59A2D6E1-E8F3-4191-89EF-C336FB7D5F26}"/>
     <cellStyle name="20% - Accent5 2" xfId="58" xr:uid="{4BB5E5F9-EFD1-45B0-90A8-FC64B00DECB1}"/>
     <cellStyle name="20% - Accent5 3" xfId="78" xr:uid="{158DEDEE-C036-4C8F-9D72-41698EA01F81}"/>
     <cellStyle name="20% - Accent5 4" xfId="98" xr:uid="{580E0739-8EA2-43A8-ABB0-A020446047A4}"/>
     <cellStyle name="20% - Accent5 5" xfId="118" xr:uid="{A0690F1E-2BA2-469B-BBF8-2CD88DC1D5B6}"/>
     <cellStyle name="20% - Accent5 6" xfId="138" xr:uid="{22CDA2E2-BB0C-415B-94E1-A625B41CBFED}"/>
     <cellStyle name="20% - Accent5 7" xfId="158" xr:uid="{469CB3C5-BFC9-4495-83E5-37AB18617440}"/>
+    <cellStyle name="20% - Accent5 8" xfId="178" xr:uid="{B51FC249-C84B-4A0F-85E6-50F31985170C}"/>
+    <cellStyle name="20% - Accent5 9" xfId="198" xr:uid="{8DFAC370-21B2-4995-90F7-7C978A7DE3CB}"/>
     <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6 10" xfId="221" xr:uid="{7512C20D-CCC3-4A72-8B33-58C3F7FB569B}"/>
     <cellStyle name="20% - Accent6 2" xfId="61" xr:uid="{A94BA87B-C4B9-42A4-B829-EEFD2D2AAEC1}"/>
     <cellStyle name="20% - Accent6 3" xfId="81" xr:uid="{3B760485-7E3C-405D-89E6-68C13D8201F6}"/>
     <cellStyle name="20% - Accent6 4" xfId="101" xr:uid="{316B90B7-455D-4097-9B9B-049F4374B448}"/>
     <cellStyle name="20% - Accent6 5" xfId="121" xr:uid="{0F5BDDE0-51CA-4409-803C-1C13A55F5C7C}"/>
     <cellStyle name="20% - Accent6 6" xfId="141" xr:uid="{59E1B5D1-2698-4589-9F02-28FE6F8ADA2F}"/>
     <cellStyle name="20% - Accent6 7" xfId="161" xr:uid="{ECC87109-A2C6-4C4A-B754-40FF7A1ED658}"/>
+    <cellStyle name="20% - Accent6 8" xfId="181" xr:uid="{32583F6C-BE5C-437D-891E-F1658A318911}"/>
+    <cellStyle name="20% - Accent6 9" xfId="201" xr:uid="{4334798D-3A15-45DC-B772-462F0BE9C951}"/>
     <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1 10" xfId="207" xr:uid="{C2EB4C88-56D8-4C51-828B-C88E7179ED44}"/>
     <cellStyle name="40% - Accent1 2" xfId="47" xr:uid="{E14EBB5E-0A47-4C48-9D86-AE1553F6599D}"/>
     <cellStyle name="40% - Accent1 3" xfId="67" xr:uid="{D7187D2C-FB59-4217-802E-DD82BD8595F1}"/>
     <cellStyle name="40% - Accent1 4" xfId="87" xr:uid="{8AE36346-8535-4E4C-8A14-2C72AFF7B9C2}"/>
     <cellStyle name="40% - Accent1 5" xfId="107" xr:uid="{3FFEBB2F-5020-4F8B-AE9A-28ED3CE43453}"/>
     <cellStyle name="40% - Accent1 6" xfId="127" xr:uid="{62E20F0B-9D7B-45AD-9870-27FF32884632}"/>
     <cellStyle name="40% - Accent1 7" xfId="147" xr:uid="{71298719-69B4-4EA3-A722-C3F5C5F98DB5}"/>
+    <cellStyle name="40% - Accent1 8" xfId="167" xr:uid="{963A2F0C-F0EC-4094-BD36-460F38108B37}"/>
+    <cellStyle name="40% - Accent1 9" xfId="187" xr:uid="{6E487329-5CE1-43B9-878A-501347BE2794}"/>
     <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2 10" xfId="210" xr:uid="{CB800431-25A8-485E-B095-5CC68BA83409}"/>
     <cellStyle name="40% - Accent2 2" xfId="50" xr:uid="{C74089CC-0A20-4656-AFB8-03E8B3304615}"/>
     <cellStyle name="40% - Accent2 3" xfId="70" xr:uid="{87D44D69-642F-4737-BACC-5522955842A3}"/>
     <cellStyle name="40% - Accent2 4" xfId="90" xr:uid="{21A1429C-BC89-4879-B848-F1E258E5D6C1}"/>
     <cellStyle name="40% - Accent2 5" xfId="110" xr:uid="{1AED2942-269D-4338-BE62-188982C8919C}"/>
     <cellStyle name="40% - Accent2 6" xfId="130" xr:uid="{CEDC178B-C707-42F8-9E91-32472E88814C}"/>
     <cellStyle name="40% - Accent2 7" xfId="150" xr:uid="{3AFC37D2-3F72-4921-9002-D8056C87BC0F}"/>
+    <cellStyle name="40% - Accent2 8" xfId="170" xr:uid="{72C411FA-EF5B-406B-AF1F-0274934F4BED}"/>
+    <cellStyle name="40% - Accent2 9" xfId="190" xr:uid="{F69EF9BD-7B90-49AB-B32B-1E88A8559205}"/>
     <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3 10" xfId="213" xr:uid="{FB289985-3714-4135-A241-8296DAF413EB}"/>
     <cellStyle name="40% - Accent3 2" xfId="53" xr:uid="{0272B091-B91F-4E63-9FBB-F7B4A6264D3F}"/>
     <cellStyle name="40% - Accent3 3" xfId="73" xr:uid="{E25EE0E1-7451-4B98-9CDD-3B48DE59DE07}"/>
     <cellStyle name="40% - Accent3 4" xfId="93" xr:uid="{95BB05CB-DA98-4F9B-A1F5-68569D0F3572}"/>
     <cellStyle name="40% - Accent3 5" xfId="113" xr:uid="{966AAB58-0070-4758-A3BD-FBE38448FC05}"/>
     <cellStyle name="40% - Accent3 6" xfId="133" xr:uid="{8B9696DA-A0B1-43F4-8748-EC191E5CD823}"/>
     <cellStyle name="40% - Accent3 7" xfId="153" xr:uid="{AEC7E618-F0DC-49A4-A941-E591E2C2754F}"/>
+    <cellStyle name="40% - Accent3 8" xfId="173" xr:uid="{A20D5DEF-756B-407E-BEA6-EF54F3C3AF48}"/>
+    <cellStyle name="40% - Accent3 9" xfId="193" xr:uid="{1445744E-90B6-488D-803E-5140EAA59A6F}"/>
     <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4 10" xfId="216" xr:uid="{E4A39A42-22FF-4E29-A91E-857C82512AF1}"/>
     <cellStyle name="40% - Accent4 2" xfId="56" xr:uid="{83EC9D9B-BEE5-470A-B080-CE16FD9AB9FA}"/>
     <cellStyle name="40% - Accent4 3" xfId="76" xr:uid="{2082F1A2-5A95-474E-B12F-9025B5FB9F11}"/>
     <cellStyle name="40% - Accent4 4" xfId="96" xr:uid="{FC4333FE-9EA6-4B82-B402-5480DF857851}"/>
     <cellStyle name="40% - Accent4 5" xfId="116" xr:uid="{FA6DFB6A-3044-436B-BD5F-85ADB642D326}"/>
     <cellStyle name="40% - Accent4 6" xfId="136" xr:uid="{419E56E7-6DDF-4D93-8840-A318CFA9CA81}"/>
     <cellStyle name="40% - Accent4 7" xfId="156" xr:uid="{E1A0704E-F894-4321-8B0F-CED2E654F9ED}"/>
+    <cellStyle name="40% - Accent4 8" xfId="176" xr:uid="{752C70F0-F54F-4127-9E1D-3F06BD2CE65A}"/>
+    <cellStyle name="40% - Accent4 9" xfId="196" xr:uid="{D7C405D6-2468-4B26-A05A-B8EDEA00CE96}"/>
     <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5 10" xfId="219" xr:uid="{95F4F69C-7793-4B51-A067-DE7E22A44152}"/>
     <cellStyle name="40% - Accent5 2" xfId="59" xr:uid="{15AD98EA-98F1-460C-85F3-BB4A4E38A363}"/>
     <cellStyle name="40% - Accent5 3" xfId="79" xr:uid="{C5480D71-5F19-44B6-B080-84766C674A1D}"/>
     <cellStyle name="40% - Accent5 4" xfId="99" xr:uid="{69745F4D-E36C-40AC-8CD0-6930986125DE}"/>
     <cellStyle name="40% - Accent5 5" xfId="119" xr:uid="{515693F2-6971-4EA6-B5D5-E989DFDB233E}"/>
     <cellStyle name="40% - Accent5 6" xfId="139" xr:uid="{47CC50E4-0CD0-4B9A-A11E-FD1501A40126}"/>
     <cellStyle name="40% - Accent5 7" xfId="159" xr:uid="{BD6A5D62-E364-48FF-BECC-87F92A5C472A}"/>
+    <cellStyle name="40% - Accent5 8" xfId="179" xr:uid="{2DEEF4E3-6F13-4C07-8F6B-7200303CEC1F}"/>
+    <cellStyle name="40% - Accent5 9" xfId="199" xr:uid="{0C8A2010-51FD-441B-AB4A-C42C30722C02}"/>
     <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6 10" xfId="222" xr:uid="{7461D848-AB54-4C39-811F-7B795B94C51F}"/>
     <cellStyle name="40% - Accent6 2" xfId="62" xr:uid="{45B59C48-4470-44FD-BB9F-F30A336F2151}"/>
     <cellStyle name="40% - Accent6 3" xfId="82" xr:uid="{7912BF9F-9C83-4653-9D16-651610831981}"/>
     <cellStyle name="40% - Accent6 4" xfId="102" xr:uid="{5515B6D7-6A40-47AC-8588-587E81DD1B3B}"/>
     <cellStyle name="40% - Accent6 5" xfId="122" xr:uid="{5AC9CC7B-EE12-4054-911D-07259C3AE937}"/>
     <cellStyle name="40% - Accent6 6" xfId="142" xr:uid="{F167FDAC-F0E4-4141-B2E0-8DFAB8921725}"/>
     <cellStyle name="40% - Accent6 7" xfId="162" xr:uid="{6FCA6D3A-662E-4469-8F62-C9320896923D}"/>
+    <cellStyle name="40% - Accent6 8" xfId="182" xr:uid="{C6EFA40F-7A28-4AA9-8221-C4887F007DC3}"/>
+    <cellStyle name="40% - Accent6 9" xfId="202" xr:uid="{F7993087-342D-4E5A-8EEE-F87C07D35C3F}"/>
     <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1 10" xfId="208" xr:uid="{2D40DE72-1A7C-4914-A3E7-013AB12191DA}"/>
     <cellStyle name="60% - Accent1 2" xfId="48" xr:uid="{E1A03B6B-FA78-45D5-939C-628EDA4E602C}"/>
     <cellStyle name="60% - Accent1 3" xfId="68" xr:uid="{5D16E2E7-DD78-4135-8AD0-5BDC88DC49AD}"/>
     <cellStyle name="60% - Accent1 4" xfId="88" xr:uid="{B1857BB0-4942-426A-9FE1-27E2795209DA}"/>
     <cellStyle name="60% - Accent1 5" xfId="108" xr:uid="{186F3E21-4265-4E50-997D-4DE1518693DB}"/>
     <cellStyle name="60% - Accent1 6" xfId="128" xr:uid="{F7071A72-0859-42A8-9A81-346C9E4C26B2}"/>
     <cellStyle name="60% - Accent1 7" xfId="148" xr:uid="{4A2E20FB-C155-4148-96DE-282CF7F995FD}"/>
+    <cellStyle name="60% - Accent1 8" xfId="168" xr:uid="{14AB3E33-AEC2-4DBA-B2E7-C8B01E4D4907}"/>
+    <cellStyle name="60% - Accent1 9" xfId="188" xr:uid="{B604F6D9-E0B7-4D09-AC4B-DB54E9F336FA}"/>
     <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2 10" xfId="211" xr:uid="{11DDA217-CFDA-41B1-A291-D1143B2236E5}"/>
     <cellStyle name="60% - Accent2 2" xfId="51" xr:uid="{D0FA212D-F77B-4084-805A-1C705D6AF2DA}"/>
     <cellStyle name="60% - Accent2 3" xfId="71" xr:uid="{B873FD5E-9C9F-4E6A-813B-AD4AECD97E71}"/>
     <cellStyle name="60% - Accent2 4" xfId="91" xr:uid="{F3C6E93D-49C0-42CD-8DBE-516F8EF9C594}"/>
     <cellStyle name="60% - Accent2 5" xfId="111" xr:uid="{3CBFB7EF-7B03-44E8-A3EC-BF3C35AE7ABE}"/>
     <cellStyle name="60% - Accent2 6" xfId="131" xr:uid="{434AB9F5-8DA9-4C0F-8B19-5ED2A3813416}"/>
     <cellStyle name="60% - Accent2 7" xfId="151" xr:uid="{D9D44644-DA90-42C1-BCA1-AFFA2F362B5A}"/>
+    <cellStyle name="60% - Accent2 8" xfId="171" xr:uid="{10A26A67-4073-4448-BEA0-F42EB1000EBB}"/>
+    <cellStyle name="60% - Accent2 9" xfId="191" xr:uid="{C8A811A0-45C3-40DD-8521-689D30F9FC9E}"/>
     <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3 10" xfId="214" xr:uid="{2CD2CD45-D144-4C3C-A9D5-61AE7DDA40F0}"/>
     <cellStyle name="60% - Accent3 2" xfId="54" xr:uid="{2DB920AF-9A1B-4809-8D7E-7E7D27029255}"/>
     <cellStyle name="60% - Accent3 3" xfId="74" xr:uid="{A793605B-7722-4F77-9376-057AEC03667C}"/>
     <cellStyle name="60% - Accent3 4" xfId="94" xr:uid="{3D5D6532-2B17-404C-BA8F-B5B4195D405A}"/>
     <cellStyle name="60% - Accent3 5" xfId="114" xr:uid="{93C42E4B-7F9E-4795-93D0-66002A0ABCAC}"/>
     <cellStyle name="60% - Accent3 6" xfId="134" xr:uid="{FDC98D8F-8FC7-41A6-96AD-E57CF63E6651}"/>
     <cellStyle name="60% - Accent3 7" xfId="154" xr:uid="{2211E40A-778C-45C7-806F-ACD77391A60B}"/>
+    <cellStyle name="60% - Accent3 8" xfId="174" xr:uid="{37B64629-2BAA-4850-AFA7-ABF0EB9780B0}"/>
+    <cellStyle name="60% - Accent3 9" xfId="194" xr:uid="{DE42D8D4-93A4-4629-8A32-E56A89008F4A}"/>
     <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4 10" xfId="217" xr:uid="{1DB35B76-39EC-4E0D-AEF6-3A94A13AE516}"/>
     <cellStyle name="60% - Accent4 2" xfId="57" xr:uid="{8195BE35-9B86-415F-9A4D-34B6410EDF5E}"/>
     <cellStyle name="60% - Accent4 3" xfId="77" xr:uid="{4CB98DF4-7B73-43E1-81E0-21FDB4DF4681}"/>
     <cellStyle name="60% - Accent4 4" xfId="97" xr:uid="{047B4172-9762-4193-8BB2-DEA383D577A2}"/>
     <cellStyle name="60% - Accent4 5" xfId="117" xr:uid="{A0CCAA26-8A16-4F5C-8643-91404041459B}"/>
     <cellStyle name="60% - Accent4 6" xfId="137" xr:uid="{5D45C577-E13B-473B-94E6-2B2DF5E03EAD}"/>
     <cellStyle name="60% - Accent4 7" xfId="157" xr:uid="{9841A7C2-752F-438C-9DFF-76E5A0DDBB81}"/>
+    <cellStyle name="60% - Accent4 8" xfId="177" xr:uid="{D704ECA8-3EF0-4F70-A21D-0393204ECA9D}"/>
+    <cellStyle name="60% - Accent4 9" xfId="197" xr:uid="{EAD3D1DC-9A29-4913-8759-C878A26794A7}"/>
     <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5 10" xfId="220" xr:uid="{70CE8811-CB9C-4B6E-95A9-FF46C0092824}"/>
     <cellStyle name="60% - Accent5 2" xfId="60" xr:uid="{2B087051-0B1A-48CB-8C88-FB5419174C45}"/>
     <cellStyle name="60% - Accent5 3" xfId="80" xr:uid="{7CA52249-2793-4CBE-9320-B2E51B7C7208}"/>
     <cellStyle name="60% - Accent5 4" xfId="100" xr:uid="{E73925E2-2A98-4246-A82E-2EB950F86CC1}"/>
     <cellStyle name="60% - Accent5 5" xfId="120" xr:uid="{5857A888-4419-4A29-BDF1-FC41D1D52AB0}"/>
     <cellStyle name="60% - Accent5 6" xfId="140" xr:uid="{CC1C09A0-3C3B-4F30-9B74-62F744EE18EF}"/>
     <cellStyle name="60% - Accent5 7" xfId="160" xr:uid="{E0C09DFE-FFC9-425D-9A04-D78059912D7A}"/>
+    <cellStyle name="60% - Accent5 8" xfId="180" xr:uid="{90AB14B9-3774-4886-B8C8-D66159501358}"/>
+    <cellStyle name="60% - Accent5 9" xfId="200" xr:uid="{18C903EB-9722-419A-92FF-E89DCA128818}"/>
     <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6 10" xfId="223" xr:uid="{99C8BEBB-7EC8-438F-97C4-BD916580407A}"/>
     <cellStyle name="60% - Accent6 2" xfId="63" xr:uid="{58557526-09F0-45A4-98F9-0C716C5F523E}"/>
     <cellStyle name="60% - Accent6 3" xfId="83" xr:uid="{E8E730DA-91DC-40A1-8E24-A1F3DDEF146E}"/>
     <cellStyle name="60% - Accent6 4" xfId="103" xr:uid="{30FF29FE-4E67-44A8-B821-3B0604D9778B}"/>
     <cellStyle name="60% - Accent6 5" xfId="123" xr:uid="{9C5609A8-B318-44B2-B52D-D6B992F316A6}"/>
     <cellStyle name="60% - Accent6 6" xfId="143" xr:uid="{CE5B77A8-D8FA-481B-8102-02F45DB1950E}"/>
     <cellStyle name="60% - Accent6 7" xfId="163" xr:uid="{1BF01C1E-7CFC-4D8A-82AF-23AE1DD8D11B}"/>
+    <cellStyle name="60% - Accent6 8" xfId="183" xr:uid="{D2EEC825-7B92-4B92-936A-947763369992}"/>
+    <cellStyle name="60% - Accent6 9" xfId="203" xr:uid="{6AE849FD-8C66-4E59-80AF-5580E35A39AD}"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
@@ -2238,6 +2385,8 @@
     <cellStyle name="Linked Cell" xfId="13" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="9" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 10" xfId="184" xr:uid="{8E6231AE-DA40-4C9E-9736-1B82EE5E5E6F}"/>
+    <cellStyle name="Normal 11" xfId="204" xr:uid="{5FC8D269-42B1-464C-968F-D78D98DD3FF3}"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{F50F2267-46E4-4CC2-A189-BCAD2533BD90}"/>
     <cellStyle name="Normal 3" xfId="44" xr:uid="{D61C6192-B0B8-490B-8EAA-C3CB05EBEB04}"/>
     <cellStyle name="Normal 4" xfId="64" xr:uid="{6E293B67-1F89-4B61-BE65-B4BC73B1F281}"/>
@@ -2245,6 +2394,9 @@
     <cellStyle name="Normal 6" xfId="104" xr:uid="{45DDF471-A5FE-4F08-AFA8-A1ABEACB6360}"/>
     <cellStyle name="Normal 7" xfId="124" xr:uid="{F6A48B77-5567-4054-914F-A75BC3F2B731}"/>
     <cellStyle name="Normal 8" xfId="144" xr:uid="{8AC7A32B-0DFC-49D9-89D1-D63994DEA6A2}"/>
+    <cellStyle name="Normal 9" xfId="164" xr:uid="{60AB3928-159E-4B63-B2EE-B9ED7592E562}"/>
+    <cellStyle name="Note 10" xfId="185" xr:uid="{00BF838E-8AEA-43DE-A47A-A73365DF3C51}"/>
+    <cellStyle name="Note 11" xfId="205" xr:uid="{D9822493-3789-448B-ADE3-0E6288BD800D}"/>
     <cellStyle name="Note 2" xfId="43" xr:uid="{1EF10F79-33D5-4582-804E-9EE3D514D4EE}"/>
     <cellStyle name="Note 3" xfId="45" xr:uid="{C97AE358-3909-487F-A4AA-9350252C81B6}"/>
     <cellStyle name="Note 4" xfId="65" xr:uid="{B117F347-10A2-45EC-8BDC-7C266E1D0FF8}"/>
@@ -2252,6 +2404,7 @@
     <cellStyle name="Note 6" xfId="105" xr:uid="{2B6C9D3B-D92B-4D19-9E71-F3A9F3DBAAB1}"/>
     <cellStyle name="Note 7" xfId="125" xr:uid="{05F74624-F17F-4C5A-8A39-E94256E41F09}"/>
     <cellStyle name="Note 8" xfId="145" xr:uid="{FED488AE-8813-4987-802B-21C9880E702F}"/>
+    <cellStyle name="Note 9" xfId="165" xr:uid="{58A36B17-87B0-42E1-B15A-475C4C53EA42}"/>
     <cellStyle name="Output" xfId="11" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Title" xfId="2" builtinId="15" customBuiltin="1"/>
@@ -3349,8 +3502,14 @@
                 <c:pt idx="1">
                   <c:v>160</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>177</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89</c:v>
+                </c:pt>
                 <c:pt idx="12" formatCode="0">
-                  <c:v>330</c:v>
+                  <c:v>596</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3700,8 +3859,14 @@
                 <c:pt idx="1">
                   <c:v>4824.1032999999979</c:v>
                 </c:pt>
+                <c:pt idx="2" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)">
+                  <c:v>5551.21</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>2546.2986000000001</c:v>
+                </c:pt>
                 <c:pt idx="12">
-                  <c:v>10390.103299999999</c:v>
+                  <c:v>18487.611899999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4258,8 +4423,14 @@
                 <c:pt idx="1">
                   <c:v>425</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>382</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>139</c:v>
+                </c:pt>
                 <c:pt idx="12">
-                  <c:v>608</c:v>
+                  <c:v>1129</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4600,8 +4771,14 @@
                 <c:pt idx="1">
                   <c:v>6429.4114000000009</c:v>
                 </c:pt>
+                <c:pt idx="2" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)">
+                  <c:v>7412.37</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)">
+                  <c:v>1909.9570999999999</c:v>
+                </c:pt>
                 <c:pt idx="12">
-                  <c:v>9433.4114000000009</c:v>
+                  <c:v>18755.738499999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7569,28 +7746,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="111"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="120"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="109" t="s">
+      <c r="L1" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="110"/>
-      <c r="P1" s="110"/>
-      <c r="Q1" s="110"/>
-      <c r="R1" s="111"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="120"/>
       <c r="S1" s="4"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
@@ -10042,8 +10219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2908758-2B63-4D19-8CDF-3000E5F1BE9C}">
   <dimension ref="A1:AX102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView topLeftCell="G83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H101" sqref="H101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10105,97 +10282,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="123" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
-      <c r="K1" s="115"/>
-      <c r="L1" s="115"/>
-      <c r="M1" s="115"/>
-      <c r="N1" s="115"/>
-      <c r="O1" s="115"/>
-      <c r="P1" s="115"/>
-      <c r="Q1" s="115"/>
-      <c r="R1" s="115"/>
-      <c r="S1" s="115"/>
-      <c r="T1" s="115"/>
-      <c r="U1" s="115"/>
-      <c r="V1" s="115"/>
-      <c r="W1" s="115"/>
-      <c r="X1" s="115"/>
-      <c r="Y1" s="115"/>
-      <c r="Z1" s="115"/>
-      <c r="AA1" s="116"/>
+      <c r="B1" s="124"/>
+      <c r="C1" s="124"/>
+      <c r="D1" s="124"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
+      <c r="G1" s="124"/>
+      <c r="H1" s="124"/>
+      <c r="I1" s="124"/>
+      <c r="J1" s="124"/>
+      <c r="K1" s="124"/>
+      <c r="L1" s="124"/>
+      <c r="M1" s="124"/>
+      <c r="N1" s="124"/>
+      <c r="O1" s="124"/>
+      <c r="P1" s="124"/>
+      <c r="Q1" s="124"/>
+      <c r="R1" s="124"/>
+      <c r="S1" s="124"/>
+      <c r="T1" s="124"/>
+      <c r="U1" s="124"/>
+      <c r="V1" s="124"/>
+      <c r="W1" s="124"/>
+      <c r="X1" s="124"/>
+      <c r="Y1" s="124"/>
+      <c r="Z1" s="124"/>
+      <c r="AA1" s="125"/>
       <c r="AB1" s="62"/>
     </row>
     <row r="2" spans="1:50" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="121" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="117" t="s">
+      <c r="C2" s="126"/>
+      <c r="D2" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="117"/>
-      <c r="F2" s="117" t="s">
+      <c r="E2" s="126"/>
+      <c r="F2" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117" t="s">
+      <c r="G2" s="126"/>
+      <c r="H2" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117" t="s">
+      <c r="I2" s="126"/>
+      <c r="J2" s="126" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="117"/>
-      <c r="L2" s="117" t="s">
+      <c r="K2" s="126"/>
+      <c r="L2" s="126" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="117"/>
-      <c r="N2" s="117" t="s">
+      <c r="M2" s="126"/>
+      <c r="N2" s="126" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="117"/>
-      <c r="P2" s="117" t="s">
+      <c r="O2" s="126"/>
+      <c r="P2" s="126" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="117"/>
-      <c r="R2" s="117" t="s">
+      <c r="Q2" s="126"/>
+      <c r="R2" s="126" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="117"/>
-      <c r="T2" s="117" t="s">
+      <c r="S2" s="126"/>
+      <c r="T2" s="126" t="s">
         <v>47</v>
       </c>
-      <c r="U2" s="117"/>
-      <c r="V2" s="117" t="s">
+      <c r="U2" s="126"/>
+      <c r="V2" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="117"/>
-      <c r="X2" s="117" t="s">
+      <c r="W2" s="126"/>
+      <c r="X2" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="117"/>
-      <c r="Z2" s="117" t="s">
+      <c r="Y2" s="126"/>
+      <c r="Z2" s="126" t="s">
         <v>168</v>
       </c>
-      <c r="AA2" s="117"/>
+      <c r="AA2" s="126"/>
       <c r="AB2" s="63"/>
     </row>
     <row r="3" spans="1:50" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="113"/>
+      <c r="A3" s="122"/>
       <c r="B3" s="38" t="s">
         <v>166</v>
       </c>
@@ -15445,10 +15622,10 @@
       <c r="C86" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D86" s="131">
+      <c r="D86" s="109">
         <v>160</v>
       </c>
-      <c r="G86" s="132">
+      <c r="G86" s="110">
         <v>4824.1032999999979</v>
       </c>
       <c r="Z86" s="79"/>
@@ -15457,11 +15634,23 @@
       <c r="C87" s="28" t="s">
         <v>30</v>
       </c>
+      <c r="D87" s="113">
+        <v>177</v>
+      </c>
+      <c r="G87" s="114">
+        <v>5551.21</v>
+      </c>
       <c r="Z87" s="79"/>
     </row>
     <row r="88" spans="3:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="28" t="s">
         <v>31</v>
+      </c>
+      <c r="D88" s="112">
+        <v>89</v>
+      </c>
+      <c r="G88" s="111">
+        <v>2546.2986000000001</v>
       </c>
       <c r="Z88" s="79"/>
     </row>
@@ -15526,11 +15715,11 @@
       </c>
       <c r="D97" s="78">
         <f>SUM(D85:D96)</f>
-        <v>330</v>
+        <v>596</v>
       </c>
       <c r="G97" s="28">
         <f>SUM(G85:G96)</f>
-        <v>10390.103299999999</v>
+        <v>18487.611899999996</v>
       </c>
       <c r="Z97" s="79"/>
     </row>
@@ -15571,7 +15760,7 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -15581,8 +15770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05395F9A-1504-413B-B37C-6F2917ED4558}">
   <dimension ref="A1:AA98"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="G87" sqref="G87"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="G89" sqref="G89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15617,95 +15806,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="127" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
-      <c r="G1" s="118"/>
-      <c r="H1" s="118"/>
-      <c r="I1" s="118"/>
-      <c r="J1" s="118"/>
-      <c r="K1" s="118"/>
-      <c r="L1" s="118"/>
-      <c r="M1" s="118"/>
-      <c r="N1" s="118"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
-      <c r="Q1" s="119"/>
-      <c r="R1" s="119"/>
-      <c r="S1" s="119"/>
-      <c r="T1" s="119"/>
-      <c r="U1" s="119"/>
-      <c r="V1" s="119"/>
-      <c r="W1" s="119"/>
-      <c r="X1" s="119"/>
-      <c r="Y1" s="119"/>
-      <c r="Z1" s="120"/>
-      <c r="AA1" s="120"/>
+      <c r="B1" s="127"/>
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
+      <c r="R1" s="128"/>
+      <c r="S1" s="128"/>
+      <c r="T1" s="128"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="128"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="128"/>
+      <c r="Y1" s="128"/>
+      <c r="Z1" s="129"/>
+      <c r="AA1" s="129"/>
     </row>
     <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="123" t="s">
+      <c r="C2" s="133"/>
+      <c r="D2" s="132" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123" t="s">
+      <c r="E2" s="132"/>
+      <c r="F2" s="132" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123" t="s">
+      <c r="G2" s="132"/>
+      <c r="H2" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123" t="s">
+      <c r="I2" s="132"/>
+      <c r="J2" s="132" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123" t="s">
+      <c r="K2" s="132"/>
+      <c r="L2" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="123"/>
-      <c r="N2" s="123" t="s">
+      <c r="M2" s="132"/>
+      <c r="N2" s="132" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="123"/>
-      <c r="P2" s="123" t="s">
+      <c r="O2" s="132"/>
+      <c r="P2" s="132" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="123"/>
-      <c r="R2" s="123" t="s">
+      <c r="Q2" s="132"/>
+      <c r="R2" s="132" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="123"/>
-      <c r="T2" s="123" t="s">
+      <c r="S2" s="132"/>
+      <c r="T2" s="132" t="s">
         <v>47</v>
       </c>
-      <c r="U2" s="123"/>
-      <c r="V2" s="123" t="s">
+      <c r="U2" s="132"/>
+      <c r="V2" s="132" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="123"/>
-      <c r="X2" s="123" t="s">
+      <c r="W2" s="132"/>
+      <c r="X2" s="132" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="123"/>
-      <c r="Z2" s="123" t="s">
+      <c r="Y2" s="132"/>
+      <c r="Z2" s="132" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="123"/>
+      <c r="AA2" s="132"/>
     </row>
     <row r="3" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="122"/>
+      <c r="A3" s="131"/>
       <c r="B3" s="26" t="s">
         <v>166</v>
       </c>
@@ -20359,10 +20548,22 @@
       <c r="C88" s="28" t="s">
         <v>30</v>
       </c>
+      <c r="D88" s="116">
+        <v>382</v>
+      </c>
+      <c r="G88" s="117">
+        <v>7412.37</v>
+      </c>
     </row>
     <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C89" s="28" t="s">
         <v>31</v>
+      </c>
+      <c r="D89" s="115">
+        <v>139</v>
+      </c>
+      <c r="G89" s="140">
+        <v>1909.9570999999999</v>
       </c>
     </row>
     <row r="90" spans="3:7" x14ac:dyDescent="0.25">
@@ -20419,11 +20620,11 @@
       </c>
       <c r="D98">
         <f>SUM(D86:D97)</f>
-        <v>608</v>
+        <v>1129</v>
       </c>
       <c r="G98" s="28">
         <f>SUM(G86:G97)</f>
-        <v>9433.4114000000009</v>
+        <v>18755.738499999999</v>
       </c>
     </row>
   </sheetData>
@@ -20444,9 +20645,10 @@
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
   </mergeCells>
-  <phoneticPr fontId="17" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -20471,63 +20673,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="137" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="128"/>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="I1" s="128" t="s">
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="135"/>
+      <c r="G1" s="135"/>
+      <c r="I1" s="137" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="129"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="138"/>
+      <c r="O1" s="138"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="130" t="s">
+      <c r="A2" s="139" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="127">
+      <c r="B2" s="136">
         <v>2020</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127">
+      <c r="C2" s="136"/>
+      <c r="D2" s="136">
         <v>2021</v>
       </c>
-      <c r="E2" s="127"/>
-      <c r="F2" s="125" t="s">
+      <c r="E2" s="136"/>
+      <c r="F2" s="134" t="s">
         <v>187</v>
       </c>
-      <c r="G2" s="127" t="s">
+      <c r="G2" s="136" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="130" t="s">
+      <c r="I2" s="139" t="s">
         <v>167</v>
       </c>
-      <c r="J2" s="127">
+      <c r="J2" s="136">
         <v>2020</v>
       </c>
-      <c r="K2" s="127"/>
-      <c r="L2" s="127">
+      <c r="K2" s="136"/>
+      <c r="L2" s="136">
         <v>2021</v>
       </c>
-      <c r="M2" s="127"/>
-      <c r="N2" s="125" t="s">
+      <c r="M2" s="136"/>
+      <c r="N2" s="134" t="s">
         <v>187</v>
       </c>
-      <c r="O2" s="127" t="s">
+      <c r="O2" s="136" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="130"/>
+      <c r="A3" s="139"/>
       <c r="B3" s="65" t="s">
         <v>1</v>
       </c>
@@ -20540,9 +20742,9 @@
       <c r="E3" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="I3" s="130"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="I3" s="139"/>
       <c r="J3" s="65" t="s">
         <v>1</v>
       </c>
@@ -20555,8 +20757,8 @@
       <c r="M3" s="65" t="s">
         <v>185</v>
       </c>
-      <c r="N3" s="126"/>
-      <c r="O3" s="126"/>
+      <c r="N3" s="135"/>
+      <c r="O3" s="135"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">

</xml_diff>

<commit_message>
Updated for July Metrics
</commit_message>
<xml_diff>
--- a/Code/Output/August_2021/Metrics_Report_August_2021.xlsx
+++ b/Code/Output/August_2021/Metrics_Report_August_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.52\home$\BryanP\Projects\project_files\USAI\Code\Output\August_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F171927-E87E-41CD-B4D3-3871E0106FA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E82696EE-3A67-4130-8274-764911282290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="3075" windowWidth="16455" windowHeight="9990" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6480" yWindow="5250" windowWidth="14100" windowHeight="6285" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Driver and Engine RMAs" sheetId="3" r:id="rId1"/>
@@ -680,10 +680,24 @@
     <numFmt numFmtId="166" formatCode="\+&quot;$&quot;0.00;\-&quot;$&quot;0.00;&quot;$&quot;0.00"/>
     <numFmt numFmtId="167" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="45" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1614,51 +1628,91 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="284">
+  <cellStyleXfs count="324">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="7" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="37" fillId="7" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="8" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="41" fillId="9" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="44" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="32" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1900,7 +1954,7 @@
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1912,16 +1966,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1944,10 +1998,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="24" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1956,7 +2010,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1971,14 +2025,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="19" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1996,7 +2050,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2005,19 +2059,19 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2036,7 +2090,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2046,10 +2100,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2067,15 +2121,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2096,7 +2150,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2111,11 +2165,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2145,7 +2199,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -2154,28 +2208,22 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="15" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="17" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="16" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2184,28 +2232,32 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="44"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="64"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="64" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="84"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="84"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="124"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="124" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="144"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="144" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="164"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="164"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="164"/>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="0" xfId="164" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="184"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="184"/>
-    <xf numFmtId="6" fontId="5" fillId="0" borderId="0" xfId="184" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="4" fillId="0" borderId="0" xfId="204" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="44"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="64"/>
+    <xf numFmtId="3" fontId="13" fillId="0" borderId="0" xfId="64" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="84"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="84"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="124"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="124" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="144"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="144" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="164"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="164"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="164"/>
+    <xf numFmtId="8" fontId="8" fillId="0" borderId="0" xfId="164" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="184"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="184"/>
+    <xf numFmtId="6" fontId="7" fillId="0" borderId="0" xfId="184" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="6" fillId="0" borderId="0" xfId="204" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="224"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="224" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="224"/>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="224" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="264"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="264" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="284" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="284"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2214,66 +2266,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="264"/>
-    <xf numFmtId="6" fontId="1" fillId="0" borderId="0" xfId="264" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="304"/>
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="304" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="284">
+  <cellStyles count="324">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent1 10" xfId="206" xr:uid="{DF50A6DA-51F4-4649-A970-1DA017078481}"/>
     <cellStyle name="20% - Accent1 11" xfId="226" xr:uid="{DA7A451B-845F-45B7-9A05-D7C5C2F9A59A}"/>
     <cellStyle name="20% - Accent1 12" xfId="246" xr:uid="{753F7579-5475-47B8-8E8F-11C14D9699E6}"/>
     <cellStyle name="20% - Accent1 13" xfId="266" xr:uid="{6AF21919-076F-44D8-8ED0-E43259700611}"/>
+    <cellStyle name="20% - Accent1 14" xfId="286" xr:uid="{9DE95A4A-5C0C-48C4-9C7F-EC2C1E7680FB}"/>
+    <cellStyle name="20% - Accent1 15" xfId="306" xr:uid="{D3AB26D6-BF14-423C-AE65-7A9D5F021255}"/>
     <cellStyle name="20% - Accent1 2" xfId="46" xr:uid="{02BAB7D6-C846-4D2A-912F-3C07D1DD4FF0}"/>
     <cellStyle name="20% - Accent1 3" xfId="66" xr:uid="{89DAF94E-6BDD-4FDC-8302-85528D01EDDA}"/>
     <cellStyle name="20% - Accent1 4" xfId="86" xr:uid="{7B1B9CF1-2737-409F-9F4B-CF269FE4FDDC}"/>
@@ -2287,6 +2341,8 @@
     <cellStyle name="20% - Accent2 11" xfId="229" xr:uid="{E0AEAD27-1B90-42DE-B9C3-983888CCCF54}"/>
     <cellStyle name="20% - Accent2 12" xfId="249" xr:uid="{3815400F-5720-4AF2-853A-CCEA8AC23822}"/>
     <cellStyle name="20% - Accent2 13" xfId="269" xr:uid="{D7DB7E40-B3B6-4897-B269-489D46B59BD7}"/>
+    <cellStyle name="20% - Accent2 14" xfId="289" xr:uid="{5BD80DD9-0DBB-4182-A1E5-6B8BD3DBE295}"/>
+    <cellStyle name="20% - Accent2 15" xfId="309" xr:uid="{137B403F-AAEF-4792-8BD3-7910D862CE22}"/>
     <cellStyle name="20% - Accent2 2" xfId="49" xr:uid="{9B8B4624-16AD-4AEE-A198-A8FDF7C8BD81}"/>
     <cellStyle name="20% - Accent2 3" xfId="69" xr:uid="{7FC42DE8-97E3-483D-86E4-1C43881206A5}"/>
     <cellStyle name="20% - Accent2 4" xfId="89" xr:uid="{6C52E251-C353-4B7E-A4FD-FEA2151429DF}"/>
@@ -2300,6 +2356,8 @@
     <cellStyle name="20% - Accent3 11" xfId="232" xr:uid="{C91DA1B2-F026-4513-A5AE-E77ABCAEB7AD}"/>
     <cellStyle name="20% - Accent3 12" xfId="252" xr:uid="{3A62E0F5-7D77-47E4-8C51-C090F83FC185}"/>
     <cellStyle name="20% - Accent3 13" xfId="272" xr:uid="{463692D0-B004-4200-9F60-26CC04F986E9}"/>
+    <cellStyle name="20% - Accent3 14" xfId="292" xr:uid="{818BDC4B-3A38-4BD4-8204-8F65AC04536D}"/>
+    <cellStyle name="20% - Accent3 15" xfId="312" xr:uid="{E0D0BCFF-685A-4E9A-9B5D-8589E508C707}"/>
     <cellStyle name="20% - Accent3 2" xfId="52" xr:uid="{7A856016-D5DC-4F33-97B8-3BDEC6B41FAE}"/>
     <cellStyle name="20% - Accent3 3" xfId="72" xr:uid="{21E79185-8EAF-4DAB-8BA0-96D4426D8503}"/>
     <cellStyle name="20% - Accent3 4" xfId="92" xr:uid="{8ACA4BD6-058B-4C3C-9972-E65B16B05DA4}"/>
@@ -2313,6 +2371,8 @@
     <cellStyle name="20% - Accent4 11" xfId="235" xr:uid="{8B654A04-8BEC-434C-A05D-9D9A655B2843}"/>
     <cellStyle name="20% - Accent4 12" xfId="255" xr:uid="{9594DDC5-7668-4F1D-BE1F-76A06FE341B4}"/>
     <cellStyle name="20% - Accent4 13" xfId="275" xr:uid="{841954DE-99A5-46FE-B575-D4D5829F3B1F}"/>
+    <cellStyle name="20% - Accent4 14" xfId="295" xr:uid="{58264A52-3800-4607-9B4E-FECC942EBD2C}"/>
+    <cellStyle name="20% - Accent4 15" xfId="315" xr:uid="{4F5F01B5-78C4-4D24-868E-6EAADDFAEBA2}"/>
     <cellStyle name="20% - Accent4 2" xfId="55" xr:uid="{27A713D1-8C98-4F40-882E-CF4BF70BE480}"/>
     <cellStyle name="20% - Accent4 3" xfId="75" xr:uid="{D490D1A2-E23D-45F5-AA9B-7EE9492D3575}"/>
     <cellStyle name="20% - Accent4 4" xfId="95" xr:uid="{56AD7626-24AD-4771-AE7E-62818455D23E}"/>
@@ -2326,6 +2386,8 @@
     <cellStyle name="20% - Accent5 11" xfId="238" xr:uid="{3E362396-D566-4F12-B157-C844EB9C42C4}"/>
     <cellStyle name="20% - Accent5 12" xfId="258" xr:uid="{EA9EE76E-585B-415C-8D51-FBF0E30923D8}"/>
     <cellStyle name="20% - Accent5 13" xfId="278" xr:uid="{34B47B4A-D340-4915-A7BA-31B83435F912}"/>
+    <cellStyle name="20% - Accent5 14" xfId="298" xr:uid="{1AA343F0-CC5F-419E-91BA-2FD3BE232A4C}"/>
+    <cellStyle name="20% - Accent5 15" xfId="318" xr:uid="{833089FB-6C0D-4DBE-B33E-F500B00DF4A9}"/>
     <cellStyle name="20% - Accent5 2" xfId="58" xr:uid="{4BB5E5F9-EFD1-45B0-90A8-FC64B00DECB1}"/>
     <cellStyle name="20% - Accent5 3" xfId="78" xr:uid="{158DEDEE-C036-4C8F-9D72-41698EA01F81}"/>
     <cellStyle name="20% - Accent5 4" xfId="98" xr:uid="{580E0739-8EA2-43A8-ABB0-A020446047A4}"/>
@@ -2339,6 +2401,8 @@
     <cellStyle name="20% - Accent6 11" xfId="241" xr:uid="{42F97139-57F4-4EE9-8546-8B480D9DCBD3}"/>
     <cellStyle name="20% - Accent6 12" xfId="261" xr:uid="{EC5133E9-23A6-45A2-8320-A1C9A516FA9E}"/>
     <cellStyle name="20% - Accent6 13" xfId="281" xr:uid="{D3C0079F-ED26-4633-8C44-77B690ECF2F0}"/>
+    <cellStyle name="20% - Accent6 14" xfId="301" xr:uid="{0C0EA01A-E585-4692-A690-F9D0155E292B}"/>
+    <cellStyle name="20% - Accent6 15" xfId="321" xr:uid="{8FFB73B6-9718-4821-B930-2E6FECA936E6}"/>
     <cellStyle name="20% - Accent6 2" xfId="61" xr:uid="{A94BA87B-C4B9-42A4-B829-EEFD2D2AAEC1}"/>
     <cellStyle name="20% - Accent6 3" xfId="81" xr:uid="{3B760485-7E3C-405D-89E6-68C13D8201F6}"/>
     <cellStyle name="20% - Accent6 4" xfId="101" xr:uid="{316B90B7-455D-4097-9B9B-049F4374B448}"/>
@@ -2352,6 +2416,8 @@
     <cellStyle name="40% - Accent1 11" xfId="227" xr:uid="{B9387841-664A-4DC1-A37B-C15A79738A35}"/>
     <cellStyle name="40% - Accent1 12" xfId="247" xr:uid="{67185ECE-B7FA-418E-8CE0-F55AF6443E5C}"/>
     <cellStyle name="40% - Accent1 13" xfId="267" xr:uid="{CB411CE9-BD3D-409E-8382-001B9F79030B}"/>
+    <cellStyle name="40% - Accent1 14" xfId="287" xr:uid="{43918641-69E5-4C34-B56A-51AF51284961}"/>
+    <cellStyle name="40% - Accent1 15" xfId="307" xr:uid="{6F5AE62D-1896-4A5C-AFDC-132BCB97A661}"/>
     <cellStyle name="40% - Accent1 2" xfId="47" xr:uid="{E14EBB5E-0A47-4C48-9D86-AE1553F6599D}"/>
     <cellStyle name="40% - Accent1 3" xfId="67" xr:uid="{D7187D2C-FB59-4217-802E-DD82BD8595F1}"/>
     <cellStyle name="40% - Accent1 4" xfId="87" xr:uid="{8AE36346-8535-4E4C-8A14-2C72AFF7B9C2}"/>
@@ -2365,6 +2431,8 @@
     <cellStyle name="40% - Accent2 11" xfId="230" xr:uid="{7BCDF6BE-DEAD-4EAB-A747-7036096D07C2}"/>
     <cellStyle name="40% - Accent2 12" xfId="250" xr:uid="{EC081CB1-D8D6-47F5-87B4-E4AD7D7487B4}"/>
     <cellStyle name="40% - Accent2 13" xfId="270" xr:uid="{16823FEF-728B-428B-8C2B-7DC3AF5B8771}"/>
+    <cellStyle name="40% - Accent2 14" xfId="290" xr:uid="{7EFBCCD1-B9B4-44DE-93E2-2A2FEAE11515}"/>
+    <cellStyle name="40% - Accent2 15" xfId="310" xr:uid="{8D23CDDC-8FD1-4B57-8412-DE89A99F47A3}"/>
     <cellStyle name="40% - Accent2 2" xfId="50" xr:uid="{C74089CC-0A20-4656-AFB8-03E8B3304615}"/>
     <cellStyle name="40% - Accent2 3" xfId="70" xr:uid="{87D44D69-642F-4737-BACC-5522955842A3}"/>
     <cellStyle name="40% - Accent2 4" xfId="90" xr:uid="{21A1429C-BC89-4879-B848-F1E258E5D6C1}"/>
@@ -2378,6 +2446,8 @@
     <cellStyle name="40% - Accent3 11" xfId="233" xr:uid="{277BFA69-773E-481D-9584-24C4F5F5D9C0}"/>
     <cellStyle name="40% - Accent3 12" xfId="253" xr:uid="{848DB2CC-B6B0-4954-8934-72A910FB4374}"/>
     <cellStyle name="40% - Accent3 13" xfId="273" xr:uid="{13CE7E19-5CF5-402D-8949-198CA66B2531}"/>
+    <cellStyle name="40% - Accent3 14" xfId="293" xr:uid="{4EC76B38-F4D2-4AE2-91E8-5D2ED410B5F7}"/>
+    <cellStyle name="40% - Accent3 15" xfId="313" xr:uid="{211EBF66-2C9A-4999-9CBE-34C2C2192F06}"/>
     <cellStyle name="40% - Accent3 2" xfId="53" xr:uid="{0272B091-B91F-4E63-9FBB-F7B4A6264D3F}"/>
     <cellStyle name="40% - Accent3 3" xfId="73" xr:uid="{E25EE0E1-7451-4B98-9CDD-3B48DE59DE07}"/>
     <cellStyle name="40% - Accent3 4" xfId="93" xr:uid="{95BB05CB-DA98-4F9B-A1F5-68569D0F3572}"/>
@@ -2391,6 +2461,8 @@
     <cellStyle name="40% - Accent4 11" xfId="236" xr:uid="{A15AB521-EDD2-4488-9B8E-B468BF725EC7}"/>
     <cellStyle name="40% - Accent4 12" xfId="256" xr:uid="{C64F4704-67C3-418C-BBBE-15B46C992F11}"/>
     <cellStyle name="40% - Accent4 13" xfId="276" xr:uid="{B5F2CEE3-D0B5-469D-89B0-760F3DE3A0BD}"/>
+    <cellStyle name="40% - Accent4 14" xfId="296" xr:uid="{4C3114AB-FE0F-4F19-B7AD-462AC5AEB7B5}"/>
+    <cellStyle name="40% - Accent4 15" xfId="316" xr:uid="{7E0F4733-A047-4B38-8440-18D8FD5FC7D4}"/>
     <cellStyle name="40% - Accent4 2" xfId="56" xr:uid="{83EC9D9B-BEE5-470A-B080-CE16FD9AB9FA}"/>
     <cellStyle name="40% - Accent4 3" xfId="76" xr:uid="{2082F1A2-5A95-474E-B12F-9025B5FB9F11}"/>
     <cellStyle name="40% - Accent4 4" xfId="96" xr:uid="{FC4333FE-9EA6-4B82-B402-5480DF857851}"/>
@@ -2404,6 +2476,8 @@
     <cellStyle name="40% - Accent5 11" xfId="239" xr:uid="{987EE0E5-97C5-4C33-88FB-5EC9B80CE386}"/>
     <cellStyle name="40% - Accent5 12" xfId="259" xr:uid="{92F800BA-3637-4C26-A741-453D0979760D}"/>
     <cellStyle name="40% - Accent5 13" xfId="279" xr:uid="{258307B7-6B3A-4BF3-BED2-A9F6F7912AC6}"/>
+    <cellStyle name="40% - Accent5 14" xfId="299" xr:uid="{89C22940-71F0-46E7-B125-728965A87C96}"/>
+    <cellStyle name="40% - Accent5 15" xfId="319" xr:uid="{68D98264-1767-4965-AC03-EFDBEDAF5E94}"/>
     <cellStyle name="40% - Accent5 2" xfId="59" xr:uid="{15AD98EA-98F1-460C-85F3-BB4A4E38A363}"/>
     <cellStyle name="40% - Accent5 3" xfId="79" xr:uid="{C5480D71-5F19-44B6-B080-84766C674A1D}"/>
     <cellStyle name="40% - Accent5 4" xfId="99" xr:uid="{69745F4D-E36C-40AC-8CD0-6930986125DE}"/>
@@ -2417,6 +2491,8 @@
     <cellStyle name="40% - Accent6 11" xfId="242" xr:uid="{81410666-474D-47BB-856E-3CCB38ADD449}"/>
     <cellStyle name="40% - Accent6 12" xfId="262" xr:uid="{89DBFF2C-62D8-4829-9BE8-CCFD25B26BE9}"/>
     <cellStyle name="40% - Accent6 13" xfId="282" xr:uid="{592AD54A-3227-4261-BEDF-C3F559E9B23B}"/>
+    <cellStyle name="40% - Accent6 14" xfId="302" xr:uid="{3EDC5033-6D5C-4976-A8DB-1221BEA120D3}"/>
+    <cellStyle name="40% - Accent6 15" xfId="322" xr:uid="{E08393D1-5AC7-464C-88AE-DF4A02FB3889}"/>
     <cellStyle name="40% - Accent6 2" xfId="62" xr:uid="{45B59C48-4470-44FD-BB9F-F30A336F2151}"/>
     <cellStyle name="40% - Accent6 3" xfId="82" xr:uid="{7912BF9F-9C83-4653-9D16-651610831981}"/>
     <cellStyle name="40% - Accent6 4" xfId="102" xr:uid="{5515B6D7-6A40-47AC-8588-587E81DD1B3B}"/>
@@ -2430,6 +2506,8 @@
     <cellStyle name="60% - Accent1 11" xfId="228" xr:uid="{7070C891-AA79-474E-8EA7-E6456EDA4DF2}"/>
     <cellStyle name="60% - Accent1 12" xfId="248" xr:uid="{CDAB397B-436D-492F-8648-379F186999DB}"/>
     <cellStyle name="60% - Accent1 13" xfId="268" xr:uid="{69D59957-84E2-4998-A73B-6539E6DA37A9}"/>
+    <cellStyle name="60% - Accent1 14" xfId="288" xr:uid="{B1B43064-7529-4D27-AF2E-F29CF1A5A093}"/>
+    <cellStyle name="60% - Accent1 15" xfId="308" xr:uid="{19AB9CAF-A3DB-46A3-929B-400C273FA34D}"/>
     <cellStyle name="60% - Accent1 2" xfId="48" xr:uid="{E1A03B6B-FA78-45D5-939C-628EDA4E602C}"/>
     <cellStyle name="60% - Accent1 3" xfId="68" xr:uid="{5D16E2E7-DD78-4135-8AD0-5BDC88DC49AD}"/>
     <cellStyle name="60% - Accent1 4" xfId="88" xr:uid="{B1857BB0-4942-426A-9FE1-27E2795209DA}"/>
@@ -2443,6 +2521,8 @@
     <cellStyle name="60% - Accent2 11" xfId="231" xr:uid="{4CCDC3AD-BF7B-4473-85F7-D5EEC3C8E251}"/>
     <cellStyle name="60% - Accent2 12" xfId="251" xr:uid="{C58B9182-3548-40EF-B84C-85D69D86CDF2}"/>
     <cellStyle name="60% - Accent2 13" xfId="271" xr:uid="{2B8D9EB6-83F5-41E1-8751-C0445B57C1C5}"/>
+    <cellStyle name="60% - Accent2 14" xfId="291" xr:uid="{AB487718-8C84-46ED-A4F9-7B426EE43382}"/>
+    <cellStyle name="60% - Accent2 15" xfId="311" xr:uid="{BFEE57D8-832F-4C74-8519-9177ACBD9C19}"/>
     <cellStyle name="60% - Accent2 2" xfId="51" xr:uid="{D0FA212D-F77B-4084-805A-1C705D6AF2DA}"/>
     <cellStyle name="60% - Accent2 3" xfId="71" xr:uid="{B873FD5E-9C9F-4E6A-813B-AD4AECD97E71}"/>
     <cellStyle name="60% - Accent2 4" xfId="91" xr:uid="{F3C6E93D-49C0-42CD-8DBE-516F8EF9C594}"/>
@@ -2456,6 +2536,8 @@
     <cellStyle name="60% - Accent3 11" xfId="234" xr:uid="{C51B81D1-6FED-40E3-A857-DE9CC22B5A88}"/>
     <cellStyle name="60% - Accent3 12" xfId="254" xr:uid="{799B7C81-7307-4232-AF89-B8DDDC9C60FE}"/>
     <cellStyle name="60% - Accent3 13" xfId="274" xr:uid="{41A4D159-08B9-4A88-AB4C-65FDD10FE416}"/>
+    <cellStyle name="60% - Accent3 14" xfId="294" xr:uid="{6737A9B6-8979-4243-A739-BC9EB6466DC8}"/>
+    <cellStyle name="60% - Accent3 15" xfId="314" xr:uid="{FFFB7EE6-C3CD-408B-9502-3D91490B5A08}"/>
     <cellStyle name="60% - Accent3 2" xfId="54" xr:uid="{2DB920AF-9A1B-4809-8D7E-7E7D27029255}"/>
     <cellStyle name="60% - Accent3 3" xfId="74" xr:uid="{A793605B-7722-4F77-9376-057AEC03667C}"/>
     <cellStyle name="60% - Accent3 4" xfId="94" xr:uid="{3D5D6532-2B17-404C-BA8F-B5B4195D405A}"/>
@@ -2469,6 +2551,8 @@
     <cellStyle name="60% - Accent4 11" xfId="237" xr:uid="{BA08DEFA-1CE2-4941-AB9C-CB09E2075C18}"/>
     <cellStyle name="60% - Accent4 12" xfId="257" xr:uid="{1D1AD600-1880-4447-9126-9ADAF9D0E5EA}"/>
     <cellStyle name="60% - Accent4 13" xfId="277" xr:uid="{F0B545A0-D0A5-48DE-B2C8-219794872A82}"/>
+    <cellStyle name="60% - Accent4 14" xfId="297" xr:uid="{D423CC0A-CDF6-43FB-8E9C-1A97A2DF9207}"/>
+    <cellStyle name="60% - Accent4 15" xfId="317" xr:uid="{AF4C1611-9084-4FC4-AA7C-9B817D6FA66F}"/>
     <cellStyle name="60% - Accent4 2" xfId="57" xr:uid="{8195BE35-9B86-415F-9A4D-34B6410EDF5E}"/>
     <cellStyle name="60% - Accent4 3" xfId="77" xr:uid="{4CB98DF4-7B73-43E1-81E0-21FDB4DF4681}"/>
     <cellStyle name="60% - Accent4 4" xfId="97" xr:uid="{047B4172-9762-4193-8BB2-DEA383D577A2}"/>
@@ -2482,6 +2566,8 @@
     <cellStyle name="60% - Accent5 11" xfId="240" xr:uid="{40088DD4-F23D-4839-BD45-D16DBBEC117F}"/>
     <cellStyle name="60% - Accent5 12" xfId="260" xr:uid="{219B4BC5-B5A0-4AFA-900D-A0B5EC1746EB}"/>
     <cellStyle name="60% - Accent5 13" xfId="280" xr:uid="{351AB47A-D826-4291-9283-813652D58C01}"/>
+    <cellStyle name="60% - Accent5 14" xfId="300" xr:uid="{3F1BA15F-8626-4E05-9396-4AF849DB3CF2}"/>
+    <cellStyle name="60% - Accent5 15" xfId="320" xr:uid="{FA876E92-EE73-4738-B35A-CEE4BD671766}"/>
     <cellStyle name="60% - Accent5 2" xfId="60" xr:uid="{2B087051-0B1A-48CB-8C88-FB5419174C45}"/>
     <cellStyle name="60% - Accent5 3" xfId="80" xr:uid="{7CA52249-2793-4CBE-9320-B2E51B7C7208}"/>
     <cellStyle name="60% - Accent5 4" xfId="100" xr:uid="{E73925E2-2A98-4246-A82E-2EB950F86CC1}"/>
@@ -2495,6 +2581,8 @@
     <cellStyle name="60% - Accent6 11" xfId="243" xr:uid="{655F3FF5-9425-4FC0-BD35-E1D4638E2D3D}"/>
     <cellStyle name="60% - Accent6 12" xfId="263" xr:uid="{592D428E-0CD2-4523-B624-ECBF8ACFA448}"/>
     <cellStyle name="60% - Accent6 13" xfId="283" xr:uid="{2EE4857A-8801-4D01-818F-57628330640E}"/>
+    <cellStyle name="60% - Accent6 14" xfId="303" xr:uid="{8C501128-7AD0-45D3-9A3A-1665FF8A9EE0}"/>
+    <cellStyle name="60% - Accent6 15" xfId="323" xr:uid="{AA65F3E4-47BA-4D5B-BEBE-FB10ED67A212}"/>
     <cellStyle name="60% - Accent6 2" xfId="63" xr:uid="{58557526-09F0-45A4-98F9-0C716C5F523E}"/>
     <cellStyle name="60% - Accent6 3" xfId="83" xr:uid="{E8E730DA-91DC-40A1-8E24-A1F3DDEF146E}"/>
     <cellStyle name="60% - Accent6 4" xfId="103" xr:uid="{30FF29FE-4E67-44A8-B821-3B0604D9778B}"/>
@@ -2527,6 +2615,8 @@
     <cellStyle name="Normal 12" xfId="224" xr:uid="{5416065E-0E58-4ED3-B31E-13774CDAE5BA}"/>
     <cellStyle name="Normal 13" xfId="244" xr:uid="{98967BAE-8BC9-469B-B6A9-65518A605B3F}"/>
     <cellStyle name="Normal 14" xfId="264" xr:uid="{32B0010D-0188-4624-AD39-9A20458E8E90}"/>
+    <cellStyle name="Normal 15" xfId="284" xr:uid="{BDB9E9ED-477A-4E89-BC15-A40E9FB0C53F}"/>
+    <cellStyle name="Normal 16" xfId="304" xr:uid="{30AD2F9F-2792-4E73-B3EB-96ABDC67B0D1}"/>
     <cellStyle name="Normal 2" xfId="42" xr:uid="{F50F2267-46E4-4CC2-A189-BCAD2533BD90}"/>
     <cellStyle name="Normal 3" xfId="44" xr:uid="{D61C6192-B0B8-490B-8EAA-C3CB05EBEB04}"/>
     <cellStyle name="Normal 4" xfId="64" xr:uid="{6E293B67-1F89-4B61-BE65-B4BC73B1F281}"/>
@@ -2540,6 +2630,8 @@
     <cellStyle name="Note 12" xfId="225" xr:uid="{EEAC6D30-30A5-4551-8C4E-6667B9DDE8C2}"/>
     <cellStyle name="Note 13" xfId="245" xr:uid="{91725AB7-4F7C-4C03-975B-DB968C9EC293}"/>
     <cellStyle name="Note 14" xfId="265" xr:uid="{B5E67E63-43A0-450C-9CF3-785C53D6CB7E}"/>
+    <cellStyle name="Note 15" xfId="285" xr:uid="{CDD3FE4E-B43F-4A6E-8694-2765F5F421AA}"/>
+    <cellStyle name="Note 16" xfId="305" xr:uid="{E04517DD-09BA-47A5-A913-244BDC9046D3}"/>
     <cellStyle name="Note 2" xfId="43" xr:uid="{1EF10F79-33D5-4582-804E-9EE3D514D4EE}"/>
     <cellStyle name="Note 3" xfId="45" xr:uid="{C97AE358-3909-487F-A4AA-9350252C81B6}"/>
     <cellStyle name="Note 4" xfId="65" xr:uid="{B117F347-10A2-45EC-8BDC-7C266E1D0FF8}"/>
@@ -3654,8 +3746,11 @@
                 <c:pt idx="4">
                   <c:v>708</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>313</c:v>
+                </c:pt>
                 <c:pt idx="12" formatCode="0">
-                  <c:v>1304</c:v>
+                  <c:v>1617</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4014,8 +4109,11 @@
                 <c:pt idx="4" formatCode="&quot;$&quot;#,##0">
                   <c:v>18482.002699999994</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>9566.8621000000003</c:v>
+                </c:pt>
                 <c:pt idx="12">
-                  <c:v>36969.614599999986</c:v>
+                  <c:v>46536.476699999985</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4581,8 +4679,11 @@
                 <c:pt idx="4">
                   <c:v>113</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>186</c:v>
+                </c:pt>
                 <c:pt idx="12">
-                  <c:v>1242</c:v>
+                  <c:v>1428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4932,8 +5033,11 @@
                 <c:pt idx="4" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)">
                   <c:v>1541</c:v>
                 </c:pt>
+                <c:pt idx="5" formatCode="&quot;$&quot;#,##0">
+                  <c:v>3122.7479999999996</c:v>
+                </c:pt>
                 <c:pt idx="12">
-                  <c:v>20296.738499999999</c:v>
+                  <c:v>23419.486499999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7901,28 +8005,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="40.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="122" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="121"/>
-      <c r="C1" s="121"/>
-      <c r="D1" s="121"/>
-      <c r="E1" s="121"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="122"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
+      <c r="E1" s="123"/>
+      <c r="F1" s="123"/>
+      <c r="G1" s="124"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="120" t="s">
+      <c r="L1" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="121"/>
-      <c r="N1" s="121"/>
-      <c r="O1" s="121"/>
-      <c r="P1" s="121"/>
-      <c r="Q1" s="121"/>
-      <c r="R1" s="122"/>
+      <c r="M1" s="123"/>
+      <c r="N1" s="123"/>
+      <c r="O1" s="123"/>
+      <c r="P1" s="123"/>
+      <c r="Q1" s="123"/>
+      <c r="R1" s="124"/>
       <c r="S1" s="4"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
@@ -8019,25 +8123,25 @@
       </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="99">
+      <c r="L3" s="97">
         <v>4</v>
       </c>
-      <c r="M3" s="99">
+      <c r="M3" s="97">
         <v>46</v>
       </c>
-      <c r="N3" s="99" t="s">
+      <c r="N3" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="O3" s="99" t="s">
+      <c r="O3" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="P3" s="100">
+      <c r="P3" s="98">
         <v>11.7</v>
       </c>
-      <c r="Q3" s="100">
+      <c r="Q3" s="98">
         <v>12.561199999999999</v>
       </c>
-      <c r="R3" s="100">
+      <c r="R3" s="98">
         <v>577.8152</v>
       </c>
       <c r="S3" s="22">
@@ -10374,8 +10478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2908758-2B63-4D19-8CDF-3000E5F1BE9C}">
   <dimension ref="A1:AX102"/>
   <sheetViews>
-    <sheetView topLeftCell="M87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView topLeftCell="A84" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G90" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10437,97 +10541,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="24.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="127" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
-      <c r="G1" s="126"/>
-      <c r="H1" s="126"/>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="126"/>
-      <c r="M1" s="126"/>
-      <c r="N1" s="126"/>
-      <c r="O1" s="126"/>
-      <c r="P1" s="126"/>
-      <c r="Q1" s="126"/>
-      <c r="R1" s="126"/>
-      <c r="S1" s="126"/>
-      <c r="T1" s="126"/>
-      <c r="U1" s="126"/>
-      <c r="V1" s="126"/>
-      <c r="W1" s="126"/>
-      <c r="X1" s="126"/>
-      <c r="Y1" s="126"/>
-      <c r="Z1" s="126"/>
-      <c r="AA1" s="127"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
+      <c r="H1" s="128"/>
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="128"/>
+      <c r="M1" s="128"/>
+      <c r="N1" s="128"/>
+      <c r="O1" s="128"/>
+      <c r="P1" s="128"/>
+      <c r="Q1" s="128"/>
+      <c r="R1" s="128"/>
+      <c r="S1" s="128"/>
+      <c r="T1" s="128"/>
+      <c r="U1" s="128"/>
+      <c r="V1" s="128"/>
+      <c r="W1" s="128"/>
+      <c r="X1" s="128"/>
+      <c r="Y1" s="128"/>
+      <c r="Z1" s="128"/>
+      <c r="AA1" s="129"/>
       <c r="AB1" s="61"/>
     </row>
     <row r="2" spans="1:50" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="123" t="s">
+      <c r="A2" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="130" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128" t="s">
+      <c r="C2" s="130"/>
+      <c r="D2" s="130" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128" t="s">
+      <c r="E2" s="130"/>
+      <c r="F2" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128" t="s">
+      <c r="G2" s="130"/>
+      <c r="H2" s="130" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128" t="s">
+      <c r="I2" s="130"/>
+      <c r="J2" s="130" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128" t="s">
+      <c r="K2" s="130"/>
+      <c r="L2" s="130" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="128"/>
-      <c r="N2" s="128" t="s">
+      <c r="M2" s="130"/>
+      <c r="N2" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="128"/>
-      <c r="P2" s="128" t="s">
+      <c r="O2" s="130"/>
+      <c r="P2" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="128"/>
-      <c r="R2" s="128" t="s">
+      <c r="Q2" s="130"/>
+      <c r="R2" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="128"/>
-      <c r="T2" s="128" t="s">
+      <c r="S2" s="130"/>
+      <c r="T2" s="130" t="s">
         <v>47</v>
       </c>
-      <c r="U2" s="128"/>
-      <c r="V2" s="128" t="s">
+      <c r="U2" s="130"/>
+      <c r="V2" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="128"/>
-      <c r="X2" s="128" t="s">
+      <c r="W2" s="130"/>
+      <c r="X2" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="128"/>
-      <c r="Z2" s="128" t="s">
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="130" t="s">
         <v>168</v>
       </c>
-      <c r="AA2" s="128"/>
+      <c r="AA2" s="130"/>
       <c r="AB2" s="62"/>
     </row>
     <row r="3" spans="1:50" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="124"/>
+      <c r="A3" s="126"/>
       <c r="B3" s="38" t="s">
         <v>166</v>
       </c>
@@ -15777,10 +15881,10 @@
       <c r="C86" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D86" s="108">
+      <c r="D86" s="106">
         <v>160</v>
       </c>
-      <c r="G86" s="109">
+      <c r="G86" s="107">
         <v>4824.1032999999979</v>
       </c>
       <c r="Z86" s="78"/>
@@ -15789,10 +15893,10 @@
       <c r="C87" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D87" s="112">
+      <c r="D87" s="110">
         <v>177</v>
       </c>
-      <c r="G87" s="113">
+      <c r="G87" s="111">
         <v>5551.21</v>
       </c>
       <c r="Z87" s="78"/>
@@ -15801,10 +15905,10 @@
       <c r="C88" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D88" s="111">
+      <c r="D88" s="109">
         <v>89</v>
       </c>
-      <c r="G88" s="110">
+      <c r="G88" s="108">
         <v>2546.2986000000001</v>
       </c>
       <c r="Z88" s="78"/>
@@ -15813,11 +15917,11 @@
       <c r="C89" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D89" s="118">
+      <c r="D89" s="116">
         <v>708</v>
       </c>
-      <c r="E89" s="119"/>
-      <c r="G89" s="119">
+      <c r="E89" s="117"/>
+      <c r="G89" s="117">
         <v>18482.002699999994</v>
       </c>
       <c r="I89" s="40"/>
@@ -15827,6 +15931,14 @@
       <c r="C90" s="28" t="s">
         <v>33</v>
       </c>
+      <c r="D90" s="121">
+        <v>313</v>
+      </c>
+      <c r="E90" s="121"/>
+      <c r="F90" s="121"/>
+      <c r="G90" s="120">
+        <v>9566.8621000000003</v>
+      </c>
       <c r="Z90" s="78"/>
     </row>
     <row r="91" spans="3:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -15853,9 +15965,9 @@
       <c r="C94" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D94" s="102"/>
-      <c r="E94" s="103"/>
-      <c r="G94" s="103"/>
+      <c r="D94" s="100"/>
+      <c r="E94" s="101"/>
+      <c r="G94" s="101"/>
       <c r="Z94" s="78"/>
     </row>
     <row r="95" spans="3:26" ht="15.75" x14ac:dyDescent="0.25">
@@ -15876,11 +15988,11 @@
       </c>
       <c r="D97" s="77">
         <f>SUM(D85:D96)</f>
-        <v>1304</v>
+        <v>1617</v>
       </c>
       <c r="G97" s="28">
         <f>SUM(G85:G96)</f>
-        <v>36969.614599999986</v>
+        <v>46536.476699999985</v>
       </c>
       <c r="Z97" s="78"/>
     </row>
@@ -15921,9 +16033,10 @@
     <mergeCell ref="N2:O2"/>
     <mergeCell ref="B2:C2"/>
   </mergeCells>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15932,7 +16045,7 @@
   <dimension ref="A1:AA98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90:G90"/>
+      <selection activeCell="D91" sqref="D91:G91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15967,95 +16080,95 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="129" t="s">
+      <c r="A1" s="131" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
-      <c r="H1" s="129"/>
-      <c r="I1" s="129"/>
-      <c r="J1" s="129"/>
-      <c r="K1" s="129"/>
-      <c r="L1" s="129"/>
-      <c r="M1" s="129"/>
-      <c r="N1" s="129"/>
-      <c r="O1" s="130"/>
-      <c r="P1" s="130"/>
-      <c r="Q1" s="130"/>
-      <c r="R1" s="130"/>
-      <c r="S1" s="130"/>
-      <c r="T1" s="130"/>
-      <c r="U1" s="130"/>
-      <c r="V1" s="130"/>
-      <c r="W1" s="130"/>
-      <c r="X1" s="130"/>
-      <c r="Y1" s="130"/>
-      <c r="Z1" s="131"/>
-      <c r="AA1" s="131"/>
+      <c r="B1" s="131"/>
+      <c r="C1" s="131"/>
+      <c r="D1" s="131"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="131"/>
+      <c r="G1" s="131"/>
+      <c r="H1" s="131"/>
+      <c r="I1" s="131"/>
+      <c r="J1" s="131"/>
+      <c r="K1" s="131"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="131"/>
+      <c r="N1" s="131"/>
+      <c r="O1" s="132"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
+      <c r="T1" s="132"/>
+      <c r="U1" s="132"/>
+      <c r="V1" s="132"/>
+      <c r="W1" s="132"/>
+      <c r="X1" s="132"/>
+      <c r="Y1" s="132"/>
+      <c r="Z1" s="133"/>
+      <c r="AA1" s="133"/>
     </row>
     <row r="2" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="134" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="134" t="s">
+      <c r="B2" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="135"/>
-      <c r="D2" s="134" t="s">
+      <c r="C2" s="137"/>
+      <c r="D2" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="134"/>
-      <c r="F2" s="134" t="s">
+      <c r="E2" s="136"/>
+      <c r="F2" s="136" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134" t="s">
+      <c r="G2" s="136"/>
+      <c r="H2" s="136" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134" t="s">
+      <c r="I2" s="136"/>
+      <c r="J2" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134" t="s">
+      <c r="K2" s="136"/>
+      <c r="L2" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134" t="s">
+      <c r="M2" s="136"/>
+      <c r="N2" s="136" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134" t="s">
+      <c r="O2" s="136"/>
+      <c r="P2" s="136" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="134"/>
-      <c r="R2" s="134" t="s">
+      <c r="Q2" s="136"/>
+      <c r="R2" s="136" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="134"/>
-      <c r="T2" s="134" t="s">
+      <c r="S2" s="136"/>
+      <c r="T2" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="U2" s="134"/>
-      <c r="V2" s="134" t="s">
+      <c r="U2" s="136"/>
+      <c r="V2" s="136" t="s">
         <v>52</v>
       </c>
-      <c r="W2" s="134"/>
-      <c r="X2" s="134" t="s">
+      <c r="W2" s="136"/>
+      <c r="X2" s="136" t="s">
         <v>62</v>
       </c>
-      <c r="Y2" s="134"/>
-      <c r="Z2" s="134" t="s">
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="136" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="134"/>
+      <c r="AA2" s="136"/>
     </row>
     <row r="3" spans="1:27" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="133"/>
+      <c r="A3" s="135"/>
       <c r="B3" s="26" t="s">
         <v>166</v>
       </c>
@@ -20698,10 +20811,10 @@
       <c r="C87" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D87" s="106">
+      <c r="D87" s="104">
         <v>425</v>
       </c>
-      <c r="G87" s="107">
+      <c r="G87" s="105">
         <v>6429.4114000000009</v>
       </c>
     </row>
@@ -20709,10 +20822,10 @@
       <c r="C88" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="D88" s="115">
+      <c r="D88" s="113">
         <v>382</v>
       </c>
-      <c r="G88" s="116">
+      <c r="G88" s="114">
         <v>7412.37</v>
       </c>
     </row>
@@ -20720,10 +20833,10 @@
       <c r="C89" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="D89" s="114">
+      <c r="D89" s="112">
         <v>139</v>
       </c>
-      <c r="G89" s="117">
+      <c r="G89" s="115">
         <v>1909.9570999999999</v>
       </c>
     </row>
@@ -20731,12 +20844,12 @@
       <c r="C90" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="D90" s="142">
+      <c r="D90" s="118">
         <v>113</v>
       </c>
-      <c r="E90" s="142"/>
-      <c r="F90" s="142"/>
-      <c r="G90" s="143">
+      <c r="E90" s="118"/>
+      <c r="F90" s="118"/>
+      <c r="G90" s="119">
         <v>1541</v>
       </c>
     </row>
@@ -20744,8 +20857,14 @@
       <c r="C91" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="D91" s="97"/>
-      <c r="G91" s="98"/>
+      <c r="D91" s="144">
+        <v>186</v>
+      </c>
+      <c r="E91" s="144"/>
+      <c r="F91" s="144"/>
+      <c r="G91" s="145">
+        <v>3122.7479999999996</v>
+      </c>
     </row>
     <row r="92" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="28" t="s">
@@ -20768,10 +20887,10 @@
       <c r="C95" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D95" s="104"/>
-      <c r="E95" s="101"/>
-      <c r="F95" s="101"/>
-      <c r="G95" s="105"/>
+      <c r="D95" s="102"/>
+      <c r="E95" s="99"/>
+      <c r="F95" s="99"/>
+      <c r="G95" s="103"/>
     </row>
     <row r="96" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C96" s="28" t="s">
@@ -20789,11 +20908,11 @@
       </c>
       <c r="D98">
         <f>SUM(D86:D97)</f>
-        <v>1242</v>
+        <v>1428</v>
       </c>
       <c r="G98" s="28">
         <f>SUM(G86:G97)</f>
-        <v>20296.738499999999</v>
+        <v>23419.486499999999</v>
       </c>
     </row>
   </sheetData>
@@ -20814,7 +20933,7 @@
     <mergeCell ref="X2:Y2"/>
     <mergeCell ref="Z2:AA2"/>
   </mergeCells>
-  <phoneticPr fontId="23" type="noConversion"/>
+  <phoneticPr fontId="25" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -20842,63 +20961,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
+      <c r="A1" s="141" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="139"/>
-      <c r="C1" s="139"/>
-      <c r="D1" s="139"/>
-      <c r="E1" s="139"/>
-      <c r="F1" s="137"/>
-      <c r="G1" s="137"/>
-      <c r="I1" s="139" t="s">
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="139"/>
+      <c r="G1" s="139"/>
+      <c r="I1" s="141" t="s">
         <v>186</v>
       </c>
-      <c r="J1" s="139"/>
-      <c r="K1" s="139"/>
-      <c r="L1" s="139"/>
-      <c r="M1" s="139"/>
-      <c r="N1" s="140"/>
-      <c r="O1" s="140"/>
+      <c r="J1" s="141"/>
+      <c r="K1" s="141"/>
+      <c r="L1" s="141"/>
+      <c r="M1" s="141"/>
+      <c r="N1" s="142"/>
+      <c r="O1" s="142"/>
     </row>
     <row r="2" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="141" t="s">
+      <c r="A2" s="143" t="s">
         <v>167</v>
       </c>
-      <c r="B2" s="138">
+      <c r="B2" s="140">
         <v>2020</v>
       </c>
-      <c r="C2" s="138"/>
-      <c r="D2" s="138">
+      <c r="C2" s="140"/>
+      <c r="D2" s="140">
         <v>2021</v>
       </c>
-      <c r="E2" s="138"/>
-      <c r="F2" s="136" t="s">
+      <c r="E2" s="140"/>
+      <c r="F2" s="138" t="s">
         <v>187</v>
       </c>
-      <c r="G2" s="138" t="s">
+      <c r="G2" s="140" t="s">
         <v>188</v>
       </c>
-      <c r="I2" s="141" t="s">
+      <c r="I2" s="143" t="s">
         <v>167</v>
       </c>
-      <c r="J2" s="138">
+      <c r="J2" s="140">
         <v>2020</v>
       </c>
-      <c r="K2" s="138"/>
-      <c r="L2" s="138">
+      <c r="K2" s="140"/>
+      <c r="L2" s="140">
         <v>2021</v>
       </c>
-      <c r="M2" s="138"/>
-      <c r="N2" s="136" t="s">
+      <c r="M2" s="140"/>
+      <c r="N2" s="138" t="s">
         <v>187</v>
       </c>
-      <c r="O2" s="138" t="s">
+      <c r="O2" s="140" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="141"/>
+      <c r="A3" s="143"/>
       <c r="B3" s="64" t="s">
         <v>1</v>
       </c>
@@ -20911,9 +21030,9 @@
       <c r="E3" s="64" t="s">
         <v>185</v>
       </c>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="I3" s="141"/>
+      <c r="F3" s="139"/>
+      <c r="G3" s="139"/>
+      <c r="I3" s="143"/>
       <c r="J3" s="64" t="s">
         <v>1</v>
       </c>
@@ -20926,8 +21045,8 @@
       <c r="M3" s="64" t="s">
         <v>185</v>
       </c>
-      <c r="N3" s="137"/>
-      <c r="O3" s="137"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="139"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="63" t="s">

</xml_diff>